<commit_message>
Ajout du MCD et MLD pour la DB_SI_SERVICE_BIBLIOTHEQUE
</commit_message>
<xml_diff>
--- a/Recapitulatif_Travaux_F2_C19_SCHLOTTER_Romain.xlsx
+++ b/Recapitulatif_Travaux_F2_C19_SCHLOTTER_Romain.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Travaux_Web_R.S._F2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BA273A-FFB7-4CED-B151-D71606869A74}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{754E9105-6DC9-4B81-9D8D-A82671F37F08}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{80263A74-2E57-4F34-B42A-6946B0F298E5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{80263A74-2E57-4F34-B42A-6946B0F298E5}"/>
   </bookViews>
   <sheets>
     <sheet name="BDD" sheetId="1" r:id="rId1"/>
@@ -666,19 +666,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -687,7 +681,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1006,7 +1006,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEB06EA7-15FC-4CC8-8804-49A41020AFB8}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
@@ -1018,14 +1018,14 @@
   <sheetData>
     <row r="1" spans="1:7" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="40"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="1:7" ht="59.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
@@ -1150,126 +1150,126 @@
       <c r="G11" s="21"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="39"/>
+      <c r="E12" s="39"/>
+      <c r="F12" s="39"/>
+      <c r="G12" s="39"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:7" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="44"/>
-      <c r="D14" s="44"/>
-      <c r="E14" s="44"/>
-      <c r="F14" s="44"/>
-      <c r="G14" s="44"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42"/>
+      <c r="E14" s="42"/>
+      <c r="F14" s="42"/>
+      <c r="G14" s="42"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="41" t="s">
+      <c r="B16" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
-      <c r="G17" s="42"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
+      <c r="F17" s="38"/>
+      <c r="G17" s="38"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="41" t="s">
+      <c r="B18" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
+      <c r="C18" s="38"/>
+      <c r="D18" s="38"/>
+      <c r="E18" s="38"/>
+      <c r="F18" s="38"/>
+      <c r="G18" s="38"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
-      <c r="G19" s="42"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
-      <c r="B20" s="41"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
+      <c r="B20" s="40"/>
+      <c r="C20" s="38"/>
+      <c r="D20" s="38"/>
+      <c r="E20" s="38"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="41"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
+      <c r="B21" s="40"/>
+      <c r="C21" s="38"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="38"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="41" t="s">
+      <c r="B22" s="40" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
+      <c r="C22" s="38"/>
+      <c r="D22" s="38"/>
+      <c r="E22" s="38"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="37"/>
@@ -1277,14 +1277,14 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="37"/>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="25" t="s">
@@ -1303,6 +1303,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
+    <mergeCell ref="B18:G18"/>
     <mergeCell ref="B24:G24"/>
     <mergeCell ref="B12:G12"/>
     <mergeCell ref="B19:G19"/>
@@ -1310,11 +1315,6 @@
     <mergeCell ref="B21:G21"/>
     <mergeCell ref="B22:G22"/>
     <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="B18:G18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1325,7 +1325,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EAD002C-45E3-477D-BBE2-5EA7E80BC117}">
   <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>

</xml_diff>